<commit_message>
edit readme in data file
</commit_message>
<xml_diff>
--- a/gapData.xlsx
+++ b/gapData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allanfriesen/TX Biomed Dropbox/Allan Friesen/rRNAdynamics/gapPaper/finalDraft/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9645C8CE-1352-614A-97C7-8397910C6BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5402B9-78B3-2241-B828-246160D5123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="840" windowWidth="24000" windowHeight="16040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="840" windowWidth="24000" windowHeight="16040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inVitro" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
     <t>Gates-BC-Rel-01_1wk_Grp 2: 2HRZE/3HR_LG C</t>
   </si>
   <si>
-    <t>This .xlsx file contains in vitro and in vivo (murine) data from experiments treating Mtb infection described in our paper, "Mind the gap: Understanding discordance between culture- and a non-culture-based measure of bacteria burden in murine tuberculosis treatment models." The data are for treatment with HRZE. In vivo data are combined from three separate experiments (experiments 3, 4, and 5), described in the methods and supplement of our paper.</t>
+    <t>This .xlsx file contains in vitro and in vivo (murine) data from experiments treating Mtb infection described in our paper, "Mind the gap: Understanding discordance between culture- and a non-culture-based measure of bacteria burden in murine tuberculosis treatment models." The data are for treatment with HRZE. In vivo data are combined from three separate experiments (experiments 3, 4, and 5), described in the methods and supplement of our paper. Note that on the inVitro tab, the 16S rRNA samples are for 50 microliters. In our code, we multiply this number by 20, to obtain counts per 1 mL.</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AC758E-504C-DD44-A05B-27789BD83EAD}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+    <sheetView zoomScale="88" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -3487,7 +3487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5A567A-711E-5842-8043-456AEC6AFB65}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
scaled data for 1 mL in datafile instead of in code
</commit_message>
<xml_diff>
--- a/gapData.xlsx
+++ b/gapData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allanfriesen/TX Biomed Dropbox/Allan Friesen/rRNAdynamics/gapPaper/finalDraft/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5402B9-78B3-2241-B828-246160D5123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5831A083-C9BD-6B44-A3CC-E55B0D6F7FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="840" windowWidth="24000" windowHeight="16040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
     <t>Gates-BC-Rel-01_1wk_Grp 2: 2HRZE/3HR_LG C</t>
   </si>
   <si>
-    <t>This .xlsx file contains in vitro and in vivo (murine) data from experiments treating Mtb infection described in our paper, "Mind the gap: Understanding discordance between culture- and a non-culture-based measure of bacteria burden in murine tuberculosis treatment models." The data are for treatment with HRZE. In vivo data are combined from three separate experiments (experiments 3, 4, and 5), described in the methods and supplement of our paper. Note that on the inVitro tab, the 16S rRNA samples are for 50 microliters. In our code, we multiply this number by 20, to obtain counts per 1 mL.</t>
+    <t>This .xlsx file contains in vitro and in vivo (murine) data from experiments treating Mtb infection described in our paper, "Mind the gap: Understanding discordance between culture- and a non-culture-based measure of bacteria burden in murine tuberculosis treatment models." The data are for treatment with HRZE. In vivo data are combined from three separate experiments (experiments 3, 4, and 5), described in the methods and supplement of our paper. In vivo CFU and 16S rRNA counts have been scaled to reflect the total mouse lung; in vitro CFU and 16S rRNA counts have been scaled to reflect 1 mL.</t>
   </si>
 </sst>
 </file>
@@ -765,10 +765,13 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -819,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>2674221707</v>
+        <v>53484434140</v>
       </c>
       <c r="H2">
         <v>67500000</v>
@@ -848,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>1743124263</v>
+        <v>34862485260</v>
       </c>
       <c r="H3">
         <v>3333333.3330000001</v>
@@ -877,7 +880,7 @@
         <v>4</v>
       </c>
       <c r="G4">
-        <v>3029516845</v>
+        <v>60590336900</v>
       </c>
       <c r="H4">
         <v>141666.6667</v>
@@ -906,7 +909,7 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>333626841.5</v>
+        <v>6672536830</v>
       </c>
       <c r="H5">
         <v>3500</v>
@@ -935,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="G6">
-        <v>25680695.899999999</v>
+        <v>513613918</v>
       </c>
       <c r="H6">
         <v>130</v>
@@ -964,7 +967,7 @@
         <v>28</v>
       </c>
       <c r="G7">
-        <v>194331.21249999999</v>
+        <v>3886624.25</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -993,7 +996,7 @@
         <v>56</v>
       </c>
       <c r="G8">
-        <v>3906.67616</v>
+        <v>78133.523199999996</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1022,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>2967008160</v>
+        <v>59340163200</v>
       </c>
       <c r="H9">
         <v>50833333.329999998</v>
@@ -1051,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <v>1892007090</v>
+        <v>37840141800</v>
       </c>
       <c r="H10">
         <v>2500000</v>
@@ -1080,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>668387882.39999998</v>
+        <v>13367757648</v>
       </c>
       <c r="H11">
         <v>116666.6667</v>
@@ -1109,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="G12">
-        <v>133968705.09999999</v>
+        <v>2679374102</v>
       </c>
       <c r="H12">
         <v>2916.666667</v>
@@ -1138,7 +1141,7 @@
         <v>14</v>
       </c>
       <c r="G13">
-        <v>13073307.310000001</v>
+        <v>261466146.20000002</v>
       </c>
       <c r="H13">
         <v>270</v>
@@ -1167,7 +1170,7 @@
         <v>28</v>
       </c>
       <c r="G14">
-        <v>299740.60239999997</v>
+        <v>5994812.0479999995</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1196,7 +1199,7 @@
         <v>56</v>
       </c>
       <c r="G15">
-        <v>33484.143660000002</v>
+        <v>669682.87320000003</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1225,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1870043616</v>
+        <v>37400872320</v>
       </c>
       <c r="H16">
         <v>55833333.329999998</v>
@@ -1254,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <v>1452749817</v>
+        <v>29054996340</v>
       </c>
       <c r="H17">
         <v>2500000</v>
@@ -1283,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="G18">
-        <v>324763200.39999998</v>
+        <v>6495264008</v>
       </c>
       <c r="H18">
         <v>266666.6667</v>
@@ -1312,7 +1315,7 @@
         <v>7</v>
       </c>
       <c r="G19">
-        <v>58417499.079999998</v>
+        <v>1168349981.5999999</v>
       </c>
       <c r="H19">
         <v>12500</v>
@@ -1341,7 +1344,7 @@
         <v>14</v>
       </c>
       <c r="G20">
-        <v>13276156.82</v>
+        <v>265523136.40000001</v>
       </c>
       <c r="H20">
         <v>220</v>
@@ -1370,7 +1373,7 @@
         <v>28</v>
       </c>
       <c r="G21">
-        <v>355068.04200000002</v>
+        <v>7101360.8399999999</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1399,7 +1402,7 @@
         <v>56</v>
       </c>
       <c r="G22">
-        <v>6410.378796</v>
+        <v>128207.57592</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1428,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>2723229378</v>
+        <v>54464587560</v>
       </c>
       <c r="H23">
         <v>38750000</v>
@@ -1457,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>3250544990</v>
+        <v>65010899800</v>
       </c>
       <c r="H24" s="1">
         <v>55000000</v>
@@ -1486,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>3219386712</v>
+        <v>64387734240</v>
       </c>
       <c r="H25">
         <v>28333333.329999998</v>
@@ -1515,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>4431185522</v>
+        <v>88623710440</v>
       </c>
       <c r="H26">
         <v>25833333.329999998</v>
@@ -1544,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>2274839036</v>
+        <v>45496780720</v>
       </c>
       <c r="H27">
         <v>31666666.670000002</v>
@@ -1573,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>2553845655</v>
+        <v>51076913100</v>
       </c>
       <c r="H28">
         <v>46666666.670000002</v>
@@ -3494,7 +3497,7 @@
     <col min="1" max="1" width="131.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="82" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>116</v>
       </c>

</xml_diff>